<commit_message>
add new time with transposed matrix
</commit_message>
<xml_diff>
--- a/ExamProject/result.xlsx
+++ b/ExamProject/result.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Parallel" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="77">
   <si>
     <t xml:space="preserve">Sequential</t>
   </si>
@@ -32,6 +32,15 @@
     <t xml:space="preserve">FF Speedup</t>
   </si>
   <si>
+    <t xml:space="preserve">Sequential trasposed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FF trasposed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FF trasposed Speedup</t>
+  </si>
+  <si>
     <t xml:space="preserve">N=1024 Thread=1, Value=339.143273</t>
   </si>
   <si>
@@ -233,116 +242,16 @@
     <t xml:space="preserve">N=10000 Processes=2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">N=10000 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Processes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">=4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">N=10000 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Processes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">=8</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">N=10000 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Processes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">=16</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">N=10000 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Processes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">=32</t>
-    </r>
+    <t xml:space="preserve">N=10000 Processes=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N=10000 Processes=8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N=10000 Processes=16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N=10000 Processes=32</t>
   </si>
 </sst>
 </file>
@@ -352,7 +261,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -373,11 +282,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -558,17 +462,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G51" activeCellId="0" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -581,11 +488,19 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0.930957</v>
@@ -597,10 +512,23 @@
         <f aca="false">B2/C2</f>
         <v>0.889217147114448</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0.16829</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>0.272738</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <f aca="false">F2/G2</f>
+        <v>0.617039063130184</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0.930957</v>
@@ -612,10 +540,23 @@
         <f aca="false">B3/C3</f>
         <v>1.52121382456702</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0.16829</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0.200718</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <f aca="false">F3/G3</f>
+        <v>0.838440000398569</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0.930957</v>
@@ -627,10 +568,23 @@
         <f aca="false">B4/C4</f>
         <v>2.46074650497062</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0.16829</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.151794</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <f aca="false">F4/G4</f>
+        <v>1.10867359711188</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0.930957</v>
@@ -642,10 +596,23 @@
         <f aca="false">B5/C5</f>
         <v>3.77903210093039</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0.16829</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0.134676</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <f aca="false">F5/G5</f>
+        <v>1.2495916124625</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>0.930957</v>
@@ -657,10 +624,23 @@
         <f aca="false">B6/C6</f>
         <v>5.09538274605103</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0.16829</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0.139719</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <f aca="false">F6/G6</f>
+        <v>1.20448901008453</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>0.930957</v>
@@ -672,6 +652,19 @@
         <f aca="false">B7/C7</f>
         <v>2.19391472795144</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0.16829</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0.250692</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <f aca="false">F7/G7</f>
+        <v>0.671301836516522</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
@@ -683,11 +676,19 @@
       <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>9.79952</v>
@@ -699,10 +700,23 @@
         <f aca="false">B9/C9</f>
         <v>1.01128045728627</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>1.45576</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <f aca="false">F9/G9</f>
+        <v>0.831888498104083</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>9.79952</v>
@@ -714,10 +728,23 @@
         <f aca="false">B10/C10</f>
         <v>1.54486637827748</v>
       </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>0.839423</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <f aca="false">F10/G10</f>
+        <v>1.44269337390088</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>9.79952</v>
@@ -729,10 +756,23 @@
         <f aca="false">B11/C11</f>
         <v>2.6786647568856</v>
       </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>0.502963</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <f aca="false">F11/G11</f>
+        <v>2.40779142799769</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>9.79952</v>
@@ -744,10 +784,23 @@
         <f aca="false">B12/C12</f>
         <v>3.81224178577264</v>
       </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>0.367459</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <f aca="false">F12/G12</f>
+        <v>3.29568741002398</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>9.79952</v>
@@ -759,10 +812,23 @@
         <f aca="false">B13/C13</f>
         <v>4.95781602566048</v>
       </c>
+      <c r="E13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>0.302929</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <f aca="false">F13/G13</f>
+        <v>3.99773544295858</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>9.79952</v>
@@ -774,10 +840,23 @@
         <f aca="false">B14/C14</f>
         <v>6.14081965158541</v>
       </c>
+      <c r="E14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>0.26466</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <f aca="false">F14/G14</f>
+        <v>4.57579536008464</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>9.79952</v>
@@ -789,10 +868,23 @@
         <f aca="false">B15/C15</f>
         <v>7.34227936493665</v>
       </c>
+      <c r="E15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>0.240502</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <f aca="false">F15/G15</f>
+        <v>5.03542590082411</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>9.79952</v>
@@ -804,10 +896,23 @@
         <f aca="false">B16/C16</f>
         <v>8.04981270946967</v>
       </c>
+      <c r="E16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>0.233063</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <f aca="false">F16/G16</f>
+        <v>5.19614868082879</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>9.79952</v>
@@ -819,10 +924,23 @@
         <f aca="false">B17/C17</f>
         <v>9.2208212578569</v>
       </c>
+      <c r="E17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>0.224124</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <f aca="false">F17/G17</f>
+        <v>5.40339276471953</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>9.79952</v>
@@ -834,10 +952,23 @@
         <f aca="false">B18/C18</f>
         <v>4.58968114204354</v>
       </c>
+      <c r="E18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>0.350696</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <f aca="false">F18/G18</f>
+        <v>3.45321874215845</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>9.79952</v>
@@ -849,10 +980,23 @@
         <f aca="false">B19/C19</f>
         <v>4.78160650330337</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>0.349926</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <f aca="false">F19/G19</f>
+        <v>3.46081742997091</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>9.79952</v>
@@ -864,10 +1008,23 @@
         <f aca="false">B20/C20</f>
         <v>5.42299795797524</v>
       </c>
+      <c r="E20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>0.332986</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <f aca="false">F20/G20</f>
+        <v>3.63687962857297</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>9.79952</v>
@@ -879,10 +1036,23 @@
         <f aca="false">B21/C21</f>
         <v>5.61509503154348</v>
       </c>
+      <c r="E21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>0.339599</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <f aca="false">F21/G21</f>
+        <v>3.56605879287042</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>9.79952</v>
@@ -894,10 +1064,23 @@
         <f aca="false">B22/C22</f>
         <v>5.97553569033013</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>0.335948</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <f aca="false">F22/G22</f>
+        <v>3.60481384023718</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>9.79952</v>
@@ -909,10 +1092,23 @@
         <f aca="false">B23/C23</f>
         <v>6.33109365309076</v>
       </c>
+      <c r="E23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>0.332417</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <f aca="false">F23/G23</f>
+        <v>3.64310489535734</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>9.79952</v>
@@ -924,10 +1120,23 @@
         <f aca="false">B24/C24</f>
         <v>6.94577775257644</v>
       </c>
+      <c r="E24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>0.336431</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <f aca="false">F24/G24</f>
+        <v>3.5996385588724</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>9.79952</v>
@@ -939,6 +1148,19 @@
         <f aca="false">B25/C25</f>
         <v>4.02450964286888</v>
       </c>
+      <c r="E25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>1.21103</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>0.470867</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <f aca="false">F25/G25</f>
+        <v>2.57191521172645</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
@@ -950,11 +1172,19 @@
       <c r="D26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>84.8628</v>
@@ -966,11 +1196,23 @@
         <f aca="false">B27/C27</f>
         <v>1.10448390573022</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>15.3747</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <f aca="false">F27/G27</f>
+        <v>0.921611478597956</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>84.8628</v>
@@ -982,11 +1224,23 @@
         <f aca="false">B28/C28</f>
         <v>1.3421626990403</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>8.70307</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <f aca="false">F28/G28</f>
+        <v>1.62810364618462</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>84.8628</v>
@@ -998,11 +1252,23 @@
         <f aca="false">B29/C29</f>
         <v>2.06600480088032</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>5.36398</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <f aca="false">F29/G29</f>
+        <v>2.64160194482455</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>84.8628</v>
@@ -1014,11 +1280,23 @@
         <f aca="false">B30/C30</f>
         <v>2.87905712802663</v>
       </c>
-      <c r="E30" s="1"/>
+      <c r="E30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>4.3659</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <f aca="false">F30/G30</f>
+        <v>3.24549348358872</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>84.8628</v>
@@ -1030,11 +1308,23 @@
         <f aca="false">B31/C31</f>
         <v>3.77693413504119</v>
       </c>
-      <c r="E31" s="1"/>
+      <c r="E31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>3.6124</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <f aca="false">F31/G31</f>
+        <v>3.9224615214262</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>84.8628</v>
@@ -1046,11 +1336,23 @@
         <f aca="false">B32/C32</f>
         <v>4.65555208110466</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>2.84268</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <f aca="false">F32/G32</f>
+        <v>4.98455682665654</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>84.8628</v>
@@ -1062,11 +1364,23 @@
         <f aca="false">B33/C33</f>
         <v>5.55693939691582</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>2.54369</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <f aca="false">F33/G33</f>
+        <v>5.57045080178795</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>84.8628</v>
@@ -1078,11 +1392,23 @@
         <f aca="false">B34/C34</f>
         <v>6.40899616348971</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>2.37174</v>
+      </c>
+      <c r="H34" s="1" t="n">
+        <f aca="false">F34/G34</f>
+        <v>5.97430578393922</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>84.8628</v>
@@ -1094,11 +1420,23 @@
         <f aca="false">B35/C35</f>
         <v>7.27561728395062</v>
       </c>
-      <c r="E35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>2.34012</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <f aca="false">F35/G35</f>
+        <v>6.05503136591286</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>84.8628</v>
@@ -1110,101 +1448,191 @@
         <f aca="false">B36/C36</f>
         <v>4.04906816294982</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>2.85323</v>
+      </c>
+      <c r="H36" s="1" t="n">
+        <f aca="false">F36/G36</f>
+        <v>4.96612610970724</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>84.8628</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C37" s="1" t="n">
         <v>20.8731</v>
       </c>
       <c r="D37" s="1" t="n">
         <f aca="false">B37/C37</f>
         <v>4.0656538798741</v>
       </c>
+      <c r="E37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G37" s="1" t="n">
+        <v>2.80334</v>
+      </c>
+      <c r="H37" s="1" t="n">
+        <f aca="false">F37/G37</f>
+        <v>5.05450641021068</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>84.8628</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C38" s="1" t="n">
         <v>19.3388</v>
       </c>
       <c r="D38" s="1" t="n">
         <f aca="false">B38/C38</f>
         <v>4.3882143669721</v>
       </c>
+      <c r="E38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>2.80937</v>
+      </c>
+      <c r="H38" s="1" t="n">
+        <f aca="false">F38/G38</f>
+        <v>5.04365747480752</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>84.8628</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39" s="1" t="n">
         <v>17.8389</v>
       </c>
       <c r="D39" s="1" t="n">
         <f aca="false">B39/C39</f>
         <v>4.75717673174916</v>
       </c>
+      <c r="E39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G39" s="1" t="n">
+        <v>2.81124</v>
+      </c>
+      <c r="H39" s="1" t="n">
+        <f aca="false">F39/G39</f>
+        <v>5.04030249996443</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>84.8628</v>
       </c>
-      <c r="C40" s="0" t="n">
+      <c r="C40" s="1" t="n">
         <v>16.7305</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">B40/C40</f>
         <v>5.07234093422193</v>
       </c>
+      <c r="E40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>2.70919</v>
+      </c>
+      <c r="H40" s="1" t="n">
+        <f aca="false">F40/G40</f>
+        <v>5.23016104444502</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>84.8628</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C41" s="1" t="n">
         <v>15.7138</v>
       </c>
       <c r="D41" s="1" t="n">
         <f aca="false">B41/C41</f>
         <v>5.40052692537769</v>
       </c>
+      <c r="E41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G41" s="1" t="n">
+        <v>2.61622</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <f aca="false">F41/G41</f>
+        <v>5.41602005947512</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>84.8628</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42" s="1" t="n">
         <v>14.8194</v>
       </c>
       <c r="D42" s="1" t="n">
         <f aca="false">B42/C42</f>
         <v>5.72646665856917</v>
       </c>
+      <c r="E42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>2.62219</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <f aca="false">F42/G42</f>
+        <v>5.40368928262254</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>84.8628</v>
@@ -1216,7 +1644,19 @@
         <f aca="false">B43/C43</f>
         <v>3.90191732953239</v>
       </c>
-      <c r="E43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G43" s="1" t="n">
+        <v>4.57889</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <f aca="false">F43/G43</f>
+        <v>3.09452727626128</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="1" t="s">
@@ -1228,11 +1668,19 @@
       <c r="D44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E44" s="1"/>
+      <c r="F44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>1053.79</v>
@@ -1244,10 +1692,23 @@
         <f aca="false">B45/C45</f>
         <v>0.926971085757514</v>
       </c>
+      <c r="E45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="G45" s="1" t="n">
+        <v>222.094</v>
+      </c>
+      <c r="H45" s="1" t="n">
+        <f aca="false">F45/G45</f>
+        <v>0.968598881554657</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>1053.79</v>
@@ -1259,10 +1720,23 @@
         <f aca="false">B46/C46</f>
         <v>1.3759115271875</v>
       </c>
+      <c r="E46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="G46" s="1" t="n">
+        <v>124.81</v>
+      </c>
+      <c r="H46" s="1" t="n">
+        <f aca="false">F46/G46</f>
+        <v>1.72357984135887</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>1053.79</v>
@@ -1274,10 +1748,23 @@
         <f aca="false">B47/C47</f>
         <v>1.91413380899532</v>
       </c>
+      <c r="E47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="G47" s="1" t="n">
+        <v>79.8601</v>
+      </c>
+      <c r="H47" s="1" t="n">
+        <f aca="false">F47/G47</f>
+        <v>2.69371062645802</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>1053.79</v>
@@ -1289,10 +1776,23 @@
         <f aca="false">B48/C48</f>
         <v>2.65404192408532</v>
       </c>
+      <c r="E48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="G48" s="1" t="n">
+        <v>56.9705</v>
+      </c>
+      <c r="H48" s="1" t="n">
+        <f aca="false">F48/G48</f>
+        <v>3.77598932781001</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>1053.79</v>
@@ -1304,11 +1804,23 @@
         <f aca="false">B49/C49</f>
         <v>4.61302410282002</v>
       </c>
-      <c r="E49" s="1"/>
+      <c r="E49" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="G49" s="1" t="n">
+        <v>36.6963</v>
+      </c>
+      <c r="H49" s="1" t="n">
+        <f aca="false">F49/G49</f>
+        <v>5.86217139057616</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>1053.79</v>
@@ -1319,6 +1831,19 @@
       <c r="D50" s="1" t="n">
         <f aca="false">B50/C50</f>
         <v>3.84464397120685</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="G50" s="1" t="n">
+        <v>62.1799</v>
+      </c>
+      <c r="H50" s="1" t="n">
+        <f aca="false">F50/G50</f>
+        <v>3.45963888652121</v>
       </c>
     </row>
   </sheetData>
@@ -1339,34 +1864,33 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>84.8628</v>
@@ -1383,7 +1907,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>84.8628</v>
@@ -1400,7 +1924,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>84.8628</v>
@@ -1417,7 +1941,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>84.8628</v>
@@ -1434,7 +1958,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>84.8628</v>
@@ -1451,7 +1975,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>84.8628</v>
@@ -1468,7 +1992,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>84.8628</v>
@@ -1485,7 +2009,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>84.8628</v>
@@ -1502,7 +2026,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>84.8628</v>
@@ -1519,7 +2043,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>84.8628</v>
@@ -1536,12 +2060,12 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>84.8628</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>41.1365</v>
       </c>
       <c r="D12" s="1" t="n">
@@ -1552,12 +2076,12 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>84.8628</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>39.9114</v>
       </c>
       <c r="D13" s="1" t="n">
@@ -1568,12 +2092,12 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>84.8628</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>38.7383</v>
       </c>
       <c r="D14" s="1" t="n">
@@ -1584,12 +2108,12 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>84.8628</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>38.3561</v>
       </c>
       <c r="D15" s="1" t="n">
@@ -1600,12 +2124,12 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>84.8628</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>38.2642</v>
       </c>
       <c r="D16" s="1" t="n">
@@ -1616,12 +2140,12 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>84.8628</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>38.3131</v>
       </c>
       <c r="D17" s="1" t="n">
@@ -1632,7 +2156,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>84.8628</v>
@@ -1648,22 +2172,21 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>1053.79</v>
@@ -1676,7 +2199,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>1053.79</v>
@@ -1689,7 +2212,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>1053.79</v>
@@ -1702,7 +2225,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>1053.79</v>
@@ -1715,7 +2238,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>1053.79</v>
@@ -1732,7 +2255,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>1053.79</v>

</xml_diff>

<commit_message>
fixed Bcast and add Allgather
</commit_message>
<xml_diff>
--- a/ExamProject/result.xlsx
+++ b/ExamProject/result.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parallel" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="77">
   <si>
     <t xml:space="preserve">Sequential</t>
   </si>
@@ -464,8 +464,8 @@
   </sheetPr>
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G51" activeCellId="0" sqref="G51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F44" activeCellId="0" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1862,10 +1862,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1873,6 +1873,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1885,8 +1889,15 @@
       <c r="D1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -1902,8 +1913,19 @@
         <f aca="false">B2/C2</f>
         <v>1.04210782255034</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>14.8103</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <f aca="false">F2/G2</f>
+        <v>0.956732814325166</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -1919,8 +1941,19 @@
         <f aca="false">B3/C3</f>
         <v>0.916436017360522</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>12.832</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <f aca="false">F3/G3</f>
+        <v>1.1042316084788</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -1936,8 +1969,19 @@
         <f aca="false">B4/C4</f>
         <v>1.59497653473367</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>12.5824</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <f aca="false">F4/G4</f>
+        <v>1.12613650813835</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -1953,8 +1997,19 @@
         <f aca="false">B5/C5</f>
         <v>2.12058922748229</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>12.924</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <f aca="false">F5/G5</f>
+        <v>1.09637109254101</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -1970,8 +2025,19 @@
         <f aca="false">B6/C6</f>
         <v>2.43027578109339</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>13.5934</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <f aca="false">F6/G6</f>
+        <v>1.04238086130034</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -1987,8 +2053,19 @@
         <f aca="false">B7/C7</f>
         <v>2.67011091009203</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>14.271</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <f aca="false">F7/G7</f>
+        <v>0.992887674304534</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -2004,8 +2081,19 @@
         <f aca="false">B8/C8</f>
         <v>2.88423342283248</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>14.8464</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <f aca="false">F8/G8</f>
+        <v>0.954406455437008</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -2021,8 +2109,19 @@
         <f aca="false">B9/C9</f>
         <v>3.09441557731226</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>14.9761</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <f aca="false">F9/G9</f>
+        <v>0.946140851089402</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -2038,8 +2137,19 @@
         <f aca="false">B10/C10</f>
         <v>3.31632629135501</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>14.4665</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <f aca="false">F10/G10</f>
+        <v>0.979469809560018</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -2055,8 +2165,19 @@
         <f aca="false">B11/C11</f>
         <v>1.99700200729025</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>18.2163</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <f aca="false">F11/G11</f>
+        <v>0.777847312571708</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -2072,7 +2193,19 @@
         <f aca="false">B12/C12</f>
         <v>2.06295625539363</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>19.2999</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <f aca="false">F12/G12</f>
+        <v>0.734174788470407</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -2088,7 +2221,19 @@
         <f aca="false">B13/C13</f>
         <v>2.12627970955667</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>20.3615</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <f aca="false">F13/G13</f>
+        <v>0.695896667730766</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -2104,7 +2249,19 @@
         <f aca="false">B14/C14</f>
         <v>2.19066918269516</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>20.5906</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <f aca="false">F14/G14</f>
+        <v>0.688153817761503</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -2120,7 +2277,19 @@
         <f aca="false">B15/C15</f>
         <v>2.2124981424076</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>21.0554</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <f aca="false">F15/G15</f>
+        <v>0.672962755397665</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -2136,7 +2305,19 @@
         <f aca="false">B16/C16</f>
         <v>2.21781194955075</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>22.1251</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <f aca="false">F16/G16</f>
+        <v>0.640426483948095</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -2152,7 +2333,19 @@
         <f aca="false">B17/C17</f>
         <v>2.21498129882468</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>23.901</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <f aca="false">F17/G17</f>
+        <v>0.592841303711142</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -2168,8 +2361,19 @@
         <f aca="false">B18/C18</f>
         <v>2.29064230881353</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>14.1695</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>23.4008</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <f aca="false">F18/G18</f>
+        <v>0.605513486718403</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
@@ -2181,8 +2385,15 @@
       <c r="D19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -2195,7 +2406,19 @@
         <f aca="false">B20/C20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>205.849</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <f aca="false">F20/G20</f>
+        <v>1.04503786756312</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -2208,7 +2431,19 @@
         <f aca="false">B21/C21</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>157.998</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <f aca="false">F21/G21</f>
+        <v>1.36153622197749</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -2221,7 +2456,19 @@
         <f aca="false">B22/C22</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>126.601</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <f aca="false">F22/G22</f>
+        <v>1.69919668880973</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -2234,7 +2481,19 @@
         <f aca="false">B23/C23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>127.184</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <f aca="false">F23/G23</f>
+        <v>1.69140772424204</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
@@ -2250,8 +2509,19 @@
         <f aca="false">B24/C24</f>
         <v>3.08375497113159</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>120.512</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <f aca="false">F24/G24</f>
+        <v>1.78505045140733</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
@@ -2264,7 +2534,19 @@
         <f aca="false">B25/C25</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>173.836</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <f aca="false">F25/G25</f>
+        <v>1.23748820727582</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add new MPI + OMP version to fix
</commit_message>
<xml_diff>
--- a/ExamProject/result.xlsx
+++ b/ExamProject/result.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="123">
   <si>
     <t xml:space="preserve">N=1024</t>
   </si>
@@ -263,6 +263,15 @@
     <t xml:space="preserve">MPI_Bcast Speedup</t>
   </si>
   <si>
+    <t xml:space="preserve">MPI_Bcast N=4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPI_Allgather N=4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPI_Allgather Speedup</t>
+  </si>
+  <si>
     <t xml:space="preserve">N=4000 Process=1, Value=1330.687030</t>
   </si>
   <si>
@@ -314,6 +323,12 @@
     <t xml:space="preserve">N=4000 Processes=32</t>
   </si>
   <si>
+    <t xml:space="preserve">MPI_Bcast N=10000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPI_Allgather N=10000 nodi=1</t>
+  </si>
+  <si>
     <t xml:space="preserve">N=10000 Process=1, Value=3330.381017</t>
   </si>
   <si>
@@ -363,6 +378,18 @@
   </si>
   <si>
     <t xml:space="preserve">N=10000 Processes=30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPI_Allgather N=10000 nodi=2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N=10000 Process=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPI_Allgather N=10000 nodi=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPI_Allgather N=10000 nodi=8</t>
   </si>
 </sst>
 </file>
@@ -1310,11 +1337,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="61322056"/>
-        <c:axId val="8135497"/>
+        <c:axId val="42743539"/>
+        <c:axId val="64853962"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61322056"/>
+        <c:axId val="42743539"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1382,7 +1409,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8135497"/>
+        <c:crossAx val="64853962"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1390,7 +1417,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8135497"/>
+        <c:axId val="64853962"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1467,7 +1494,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61322056"/>
+        <c:crossAx val="42743539"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1519,6 +1546,1006 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:rPr>
+              <a:t>Distributed speedup with MPI</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0784390135278072"/>
+          <c:y val="0.172592237661715"/>
+          <c:w val="0.690474865000278"/>
+          <c:h val="0.586200287494011"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Distributed!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MPI_Bcast N=4000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Distributed!$K$2:$K$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Distributed!$H$2:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.956732814325166</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1042316084788</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.12613650813835</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.09637109254101</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.04238086130034</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.992887674304534</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.954406455437008</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.946140851089402</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.979469809560018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.777847312571708</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.734174788470407</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.695896667730766</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.688153817761503</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.672962755397665</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.640426483948095</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.592841303711142</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.605513486718403</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Distributed!$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MPI_Bcast N=10000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Distributed!$K$2:$K$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Distributed!$H$20:$H$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1.04503786756312</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.36153622197749</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.69919668880973</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.73024797110891</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.69140772424204</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.69289851422815</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.72555688353774</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.77234379119431</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.78505045140733</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.45545083658654</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.39210115900575</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.37506072460433</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.35591511033513</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.32927153300007</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.26555320888805</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.22861826136124</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.23748820727582</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Distributed!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MPI_Allgather N=4000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Distributed!$K$2:$K$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Distributed!$J$2:$J$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1.00768771246106</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.58004016588219</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.38873529114266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.58952639418113</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.48451289029007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.96071945723103</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.41392603300807</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.83423713036325</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.38495508124986</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.2254503156136</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.31769256524987</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.12049912129634</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.06305313082314</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.01969584601352</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.88533396322851</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.80373739312476</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.82694007353895</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Distributed!$I$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MPI_Allgather N=10000 nodi=1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Distributed!$K$2:$K$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Distributed!$J$20:$J$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.975295712452793</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.69407169407169</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.61338814742464</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8922764172988</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.85511789704481</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.44612151134663</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.92715270475523</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.35566984216974</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.80860147754071</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.51602084245899</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.8116433016287</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.92387908060989</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.93429191158451</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.98174232692785</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.0171802054155</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.94262736746416</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.85940235956024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="80125511"/>
+        <c:axId val="47142580"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="80125511"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
+                  </a:rPr>
+                  <a:t>Number of processes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="47142580"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="47142580"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
+                  </a:rPr>
+                  <a:t>Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="80125511"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.794445062896583"/>
+          <c:y val="0.196110365970492"/>
+          <c:w val="0.193309584771235"/>
+          <c:h val="0.557578080091972"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -1530,9 +2557,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>175680</xdr:colOff>
+      <xdr:colOff>173880</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>16920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1541,7 +2568,42 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12143520" y="1329120"/>
-        <a:ext cx="5754960" cy="3241440"/>
+        <a:ext cx="5753160" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>154800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>118800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>55800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="16994520" y="200880"/>
+        <a:ext cx="6466320" cy="3756240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1667,7 +2729,7 @@
   </sheetPr>
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="S14" activeCellId="0" sqref="S14"/>
     </sheetView>
   </sheetViews>
@@ -3543,10 +4605,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I57" activeCellId="0" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3557,7 +4619,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="27.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.03"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3574,15 +4638,21 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>84.8628</v>
@@ -3595,7 +4665,7 @@
         <v>1.04210782255034</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>14.1695</v>
@@ -3607,10 +4677,20 @@
         <f aca="false">F2/G2</f>
         <v>0.956732814325166</v>
       </c>
+      <c r="I2" s="1" t="n">
+        <v>14.0614</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <f aca="false">F2/I2</f>
+        <v>1.00768771246106</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>84.8628</v>
@@ -3623,7 +4703,7 @@
         <v>0.916436017360522</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>14.1695</v>
@@ -3635,10 +4715,20 @@
         <f aca="false">F3/G3</f>
         <v>1.1042316084788</v>
       </c>
+      <c r="I3" s="1" t="n">
+        <v>8.96781</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <f aca="false">F3/I3</f>
+        <v>1.58004016588219</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>84.8628</v>
@@ -3651,7 +4741,7 @@
         <v>1.59497653473367</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>14.1695</v>
@@ -3663,10 +4753,20 @@
         <f aca="false">F4/G4</f>
         <v>1.12613650813835</v>
       </c>
+      <c r="I4" s="1" t="n">
+        <v>5.9318</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <f aca="false">F4/I4</f>
+        <v>2.38873529114266</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>84.8628</v>
@@ -3679,7 +4779,7 @@
         <v>2.12058922748229</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>14.1695</v>
@@ -3691,10 +4791,20 @@
         <f aca="false">F5/G5</f>
         <v>1.09637109254101</v>
       </c>
+      <c r="I5" s="1" t="n">
+        <v>5.47185</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <f aca="false">F5/I5</f>
+        <v>2.58952639418113</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>84.8628</v>
@@ -3707,7 +4817,7 @@
         <v>2.43027578109339</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>14.1695</v>
@@ -3719,10 +4829,20 @@
         <f aca="false">F6/G6</f>
         <v>1.04238086130034</v>
       </c>
+      <c r="I6" s="1" t="n">
+        <v>5.70313</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <f aca="false">F6/I6</f>
+        <v>2.48451289029007</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>84.8628</v>
@@ -3735,7 +4855,7 @@
         <v>2.67011091009203</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>14.1695</v>
@@ -3747,10 +4867,20 @@
         <f aca="false">F7/G7</f>
         <v>0.992887674304534</v>
       </c>
+      <c r="I7" s="1" t="n">
+        <v>4.78583</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <f aca="false">F7/I7</f>
+        <v>2.96071945723103</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>84.8628</v>
@@ -3763,7 +4893,7 @@
         <v>2.88423342283248</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>14.1695</v>
@@ -3775,10 +4905,20 @@
         <f aca="false">F8/G8</f>
         <v>0.954406455437008</v>
       </c>
+      <c r="I8" s="1" t="n">
+        <v>4.1505</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <f aca="false">F8/I8</f>
+        <v>3.41392603300807</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>84.8628</v>
@@ -3791,7 +4931,7 @@
         <v>3.09441557731226</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>14.1695</v>
@@ -3803,10 +4943,20 @@
         <f aca="false">F9/G9</f>
         <v>0.946140851089402</v>
       </c>
+      <c r="I9" s="1" t="n">
+        <v>3.69552</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <f aca="false">F9/I9</f>
+        <v>3.83423713036325</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>84.8628</v>
@@ -3819,7 +4969,7 @@
         <v>3.31632629135501</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>14.1695</v>
@@ -3831,10 +4981,20 @@
         <f aca="false">F10/G10</f>
         <v>0.979469809560018</v>
       </c>
+      <c r="I10" s="1" t="n">
+        <v>3.23139</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <f aca="false">F10/I10</f>
+        <v>4.38495508124986</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>84.8628</v>
@@ -3847,7 +5007,7 @@
         <v>1.99700200729025</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>14.1695</v>
@@ -3859,10 +5019,20 @@
         <f aca="false">F11/G11</f>
         <v>0.777847312571708</v>
       </c>
+      <c r="I11" s="1" t="n">
+        <v>4.39303</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <f aca="false">F11/I11</f>
+        <v>3.2254503156136</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>84.8628</v>
@@ -3875,7 +5045,7 @@
         <v>2.06295625539363</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>14.1695</v>
@@ -3887,10 +5057,20 @@
         <f aca="false">F12/G12</f>
         <v>0.734174788470407</v>
       </c>
+      <c r="I12" s="1" t="n">
+        <v>4.27089</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <f aca="false">F12/I12</f>
+        <v>3.31769256524987</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>84.8628</v>
@@ -3903,7 +5083,7 @@
         <v>2.12627970955667</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F13" s="1" t="n">
         <v>14.1695</v>
@@ -3915,10 +5095,20 @@
         <f aca="false">F13/G13</f>
         <v>0.695896667730766</v>
       </c>
+      <c r="I13" s="1" t="n">
+        <v>4.54078</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <f aca="false">F13/I13</f>
+        <v>3.12049912129634</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>84.8628</v>
@@ -3931,7 +5121,7 @@
         <v>2.19066918269516</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>14.1695</v>
@@ -3943,10 +5133,20 @@
         <f aca="false">F14/G14</f>
         <v>0.688153817761503</v>
       </c>
+      <c r="I14" s="1" t="n">
+        <v>4.62594</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <f aca="false">F14/I14</f>
+        <v>3.06305313082314</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>84.8628</v>
@@ -3959,7 +5159,7 @@
         <v>2.2124981424076</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>14.1695</v>
@@ -3971,10 +5171,20 @@
         <f aca="false">F15/G15</f>
         <v>0.672962755397665</v>
       </c>
+      <c r="I15" s="1" t="n">
+        <v>4.69236</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <f aca="false">F15/I15</f>
+        <v>3.01969584601352</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>84.8628</v>
@@ -3987,7 +5197,7 @@
         <v>2.21781194955075</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F16" s="1" t="n">
         <v>14.1695</v>
@@ -3999,10 +5209,20 @@
         <f aca="false">F16/G16</f>
         <v>0.640426483948095</v>
       </c>
+      <c r="I16" s="1" t="n">
+        <v>4.91087</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <f aca="false">F16/I16</f>
+        <v>2.88533396322851</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>84.8628</v>
@@ -4015,7 +5235,7 @@
         <v>2.21498129882468</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>14.1695</v>
@@ -4027,10 +5247,20 @@
         <f aca="false">F17/G17</f>
         <v>0.592841303711142</v>
       </c>
+      <c r="I17" s="1" t="n">
+        <v>5.05379</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <f aca="false">F17/I17</f>
+        <v>2.80373739312476</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>84.8628</v>
@@ -4043,7 +5273,7 @@
         <v>2.29064230881353</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>14.1695</v>
@@ -4055,6 +5285,16 @@
         <f aca="false">F18/G18</f>
         <v>0.605513486718403</v>
       </c>
+      <c r="I18" s="1" t="n">
+        <v>5.01231</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <f aca="false">F18/I18</f>
+        <v>2.82694007353895</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
@@ -4070,15 +5310,21 @@
         <v>4</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="I19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>1053.79</v>
@@ -4088,7 +5334,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>215.12</v>
@@ -4100,10 +5346,17 @@
         <f aca="false">F20/G20</f>
         <v>1.04503786756312</v>
       </c>
+      <c r="I20" s="1" t="n">
+        <v>220.569</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <f aca="false">F20/I20</f>
+        <v>0.975295712452793</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>1053.79</v>
@@ -4113,7 +5366,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F21" s="1" t="n">
         <v>215.12</v>
@@ -4125,10 +5378,17 @@
         <f aca="false">F21/G21</f>
         <v>1.36153622197749</v>
       </c>
+      <c r="I21" s="1" t="n">
+        <v>126.984</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <f aca="false">F21/I21</f>
+        <v>1.69407169407169</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>1053.79</v>
@@ -4138,7 +5398,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F22" s="1" t="n">
         <v>215.12</v>
@@ -4150,10 +5410,17 @@
         <f aca="false">F22/G22</f>
         <v>1.69919668880973</v>
       </c>
+      <c r="I22" s="1" t="n">
+        <v>82.3146</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <f aca="false">F22/I22</f>
+        <v>2.61338814742464</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>1053.79</v>
@@ -4163,22 +5430,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>215.12</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="G23" s="1" t="n">
         <v>124.329</v>
       </c>
       <c r="H23" s="1" t="n">
         <f aca="false">F23/G23</f>
         <v>1.73024797110891</v>
       </c>
+      <c r="I23" s="1" t="n">
+        <v>74.3774</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <f aca="false">F23/I23</f>
+        <v>2.8922764172988</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>1053.79</v>
@@ -4191,7 +5465,7 @@
         <v>3.08375497113159</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F24" s="1" t="n">
         <v>215.12</v>
@@ -4203,10 +5477,17 @@
         <f aca="false">F24/G24</f>
         <v>1.69140772424204</v>
       </c>
+      <c r="I24" s="1" t="n">
+        <v>75.3454</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <f aca="false">F24/I24</f>
+        <v>2.85511789704481</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>1053.79</v>
@@ -4216,22 +5497,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="F25" s="1" t="n">
         <v>215.12</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="1" t="n">
         <v>127.072</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">F25/G25</f>
         <v>1.69289851422815</v>
       </c>
+      <c r="I25" s="1" t="n">
+        <v>62.4238</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <f aca="false">F25/I25</f>
+        <v>3.44612151134663</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F26" s="1" t="n">
         <v>215.12</v>
@@ -4243,10 +5531,17 @@
         <f aca="false">F26/G26</f>
         <v>1.72555688353774</v>
       </c>
+      <c r="I26" s="1" t="n">
+        <v>54.7776</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <f aca="false">F26/I26</f>
+        <v>3.92715270475523</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>215.12</v>
@@ -4258,10 +5553,17 @@
         <f aca="false">F27/G27</f>
         <v>1.77234379119431</v>
       </c>
+      <c r="I27" s="1" t="n">
+        <v>49.3885</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <f aca="false">F27/I27</f>
+        <v>4.35566984216974</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F28" s="1" t="n">
         <v>215.12</v>
@@ -4273,10 +5575,17 @@
         <f aca="false">F28/G28</f>
         <v>1.78505045140733</v>
       </c>
+      <c r="I28" s="1" t="n">
+        <v>44.7365</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <f aca="false">F28/I28</f>
+        <v>4.80860147754071</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="F29" s="1" t="n">
         <v>215.12</v>
@@ -4288,10 +5597,17 @@
         <f aca="false">F29/G29</f>
         <v>1.45545083658654</v>
       </c>
+      <c r="I29" s="1" t="n">
+        <v>61.1828</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <f aca="false">F29/I29</f>
+        <v>3.51602084245899</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F30" s="1" t="n">
         <v>215.12</v>
@@ -4303,10 +5619,17 @@
         <f aca="false">F30/G30</f>
         <v>1.39210115900575</v>
       </c>
+      <c r="I30" s="1" t="n">
+        <v>56.4376</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <f aca="false">F30/I30</f>
+        <v>3.8116433016287</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F31" s="1" t="n">
         <v>215.12</v>
@@ -4318,10 +5641,17 @@
         <f aca="false">F31/G31</f>
         <v>1.37506072460433</v>
       </c>
+      <c r="I31" s="1" t="n">
+        <v>54.8233</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <f aca="false">F31/I31</f>
+        <v>3.92387908060989</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F32" s="1" t="n">
         <v>215.12</v>
@@ -4333,10 +5663,17 @@
         <f aca="false">F32/G32</f>
         <v>1.35591511033513</v>
       </c>
+      <c r="I32" s="1" t="n">
+        <v>54.6782</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <f aca="false">F32/I32</f>
+        <v>3.93429191158451</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F33" s="1" t="n">
         <v>215.12</v>
@@ -4348,10 +5685,17 @@
         <f aca="false">F33/G33</f>
         <v>1.32927153300007</v>
       </c>
+      <c r="I33" s="1" t="n">
+        <v>54.0266</v>
+      </c>
+      <c r="J33" s="2" t="n">
+        <f aca="false">F33/I33</f>
+        <v>3.98174232692785</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F34" s="1" t="n">
         <v>215.12</v>
@@ -4363,10 +5707,17 @@
         <f aca="false">F34/G34</f>
         <v>1.26555320888805</v>
       </c>
+      <c r="I34" s="1" t="n">
+        <v>53.55</v>
+      </c>
+      <c r="J34" s="2" t="n">
+        <f aca="false">F34/I34</f>
+        <v>4.0171802054155</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="F35" s="1" t="n">
         <v>215.12</v>
@@ -4378,10 +5729,17 @@
         <f aca="false">F35/G35</f>
         <v>1.22861826136124</v>
       </c>
+      <c r="I35" s="1" t="n">
+        <v>54.5626</v>
+      </c>
+      <c r="J35" s="2" t="n">
+        <f aca="false">F35/I35</f>
+        <v>3.94262736746416</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F36" s="1" t="n">
         <v>215.12</v>
@@ -4393,24 +5751,793 @@
         <f aca="false">F36/G36</f>
         <v>1.23748820727582</v>
       </c>
+      <c r="I36" s="1" t="n">
+        <v>55.7392</v>
+      </c>
+      <c r="J36" s="2" t="n">
+        <f aca="false">F36/I36</f>
+        <v>3.85940235956024</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I37" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F38" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>235.456</v>
+      </c>
+      <c r="J38" s="2" t="n">
+        <f aca="false">F38/I38</f>
+        <v>0.913631421581952</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F39" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>124.822</v>
+      </c>
+      <c r="J39" s="2" t="n">
+        <f aca="false">F39/I39</f>
+        <v>1.72341414173783</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E40" s="0"/>
-      <c r="F40" s="0"/>
-      <c r="G40" s="0"/>
-      <c r="H40" s="0"/>
+      <c r="F40" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>82.2214</v>
+      </c>
+      <c r="J40" s="2" t="n">
+        <f aca="false">F40/I40</f>
+        <v>2.6163504878292</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E41" s="0"/>
-      <c r="F41" s="0"/>
-      <c r="G41" s="0"/>
-      <c r="H41" s="0"/>
+      <c r="F41" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>75.8462</v>
+      </c>
+      <c r="J41" s="2" t="n">
+        <f aca="false">F41/I41</f>
+        <v>2.83626602255617</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E42" s="0"/>
-      <c r="F42" s="0"/>
-      <c r="G42" s="0"/>
-      <c r="H42" s="0"/>
+      <c r="F42" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <v>75.5354</v>
+      </c>
+      <c r="J42" s="2" t="n">
+        <f aca="false">F42/I42</f>
+        <v>2.84793619945085</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F43" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <v>62.667</v>
+      </c>
+      <c r="J43" s="2" t="n">
+        <f aca="false">F43/I43</f>
+        <v>3.43274769815054</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F44" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I44" s="1" t="n">
+        <v>54.868</v>
+      </c>
+      <c r="J44" s="2" t="n">
+        <f aca="false">F44/I44</f>
+        <v>3.9206823649486</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F45" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>48.9448</v>
+      </c>
+      <c r="J45" s="2" t="n">
+        <f aca="false">F45/I45</f>
+        <v>4.39515535868979</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F46" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <v>45.3164</v>
+      </c>
+      <c r="J46" s="2" t="n">
+        <f aca="false">F46/I46</f>
+        <v>4.74706728689834</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F47" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>60.7967</v>
+      </c>
+      <c r="J47" s="2" t="n">
+        <f aca="false">F47/I47</f>
+        <v>3.53834994333574</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F48" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I48" s="1" t="n">
+        <v>58.5514</v>
+      </c>
+      <c r="J48" s="2" t="n">
+        <f aca="false">F48/I48</f>
+        <v>3.67403682917915</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F49" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I49" s="1" t="n">
+        <v>55.166</v>
+      </c>
+      <c r="J49" s="2" t="n">
+        <f aca="false">F49/I49</f>
+        <v>3.89950331726063</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F50" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I50" s="1" t="n">
+        <v>52.6764</v>
+      </c>
+      <c r="J50" s="2" t="n">
+        <f aca="false">F50/I50</f>
+        <v>4.08380223401751</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F51" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I51" s="1" t="n">
+        <v>52.1187</v>
+      </c>
+      <c r="J51" s="2" t="n">
+        <f aca="false">F51/I51</f>
+        <v>4.12750126154336</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F52" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I52" s="1" t="n">
+        <v>56.1365</v>
+      </c>
+      <c r="J52" s="2" t="n">
+        <f aca="false">F52/I52</f>
+        <v>3.83208785727646</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F53" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I53" s="1" t="n">
+        <v>57.7841</v>
+      </c>
+      <c r="J53" s="2" t="n">
+        <f aca="false">F53/I53</f>
+        <v>3.7228234064388</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F54" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I54" s="1" t="n">
+        <v>56.2831</v>
+      </c>
+      <c r="J54" s="2" t="n">
+        <f aca="false">F54/I54</f>
+        <v>3.82210645824413</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I55" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F56" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I56" s="1" t="n">
+        <v>220.439</v>
+      </c>
+      <c r="J56" s="2" t="n">
+        <f aca="false">F56/I56</f>
+        <v>0.975870875843204</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F57" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I57" s="1" t="n">
+        <v>133.685</v>
+      </c>
+      <c r="J57" s="2" t="n">
+        <f aca="false">F57/I57</f>
+        <v>1.60915585144182</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F58" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I58" s="1" t="n">
+        <v>82.5335</v>
+      </c>
+      <c r="J58" s="2" t="n">
+        <f aca="false">F58/I58</f>
+        <v>2.6064567720986</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F59" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I59" s="1" t="n">
+        <v>75.4285</v>
+      </c>
+      <c r="J59" s="2" t="n">
+        <f aca="false">F59/I59</f>
+        <v>2.85197239770113</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F60" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I60" s="1" t="n">
+        <v>75.2375</v>
+      </c>
+      <c r="J60" s="2" t="n">
+        <f aca="false">F60/I60</f>
+        <v>2.85921249376973</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F61" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I61" s="1" t="n">
+        <v>62.233</v>
+      </c>
+      <c r="J61" s="2" t="n">
+        <f aca="false">F61/I61</f>
+        <v>3.45668696672184</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F62" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I62" s="1" t="n">
+        <v>55.0611</v>
+      </c>
+      <c r="J62" s="2" t="n">
+        <f aca="false">F62/I62</f>
+        <v>3.90693248046261</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F63" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I63" s="1" t="n">
+        <v>49.0801</v>
+      </c>
+      <c r="J63" s="2" t="n">
+        <f aca="false">F63/I63</f>
+        <v>4.38303915436195</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F64" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I64" s="1" t="n">
+        <v>45.0207</v>
+      </c>
+      <c r="J64" s="2" t="n">
+        <f aca="false">F64/I64</f>
+        <v>4.77824645107695</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F65" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I65" s="1" t="n">
+        <v>58.7625</v>
+      </c>
+      <c r="J65" s="2" t="n">
+        <f aca="false">F65/I65</f>
+        <v>3.66083811954903</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F66" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I66" s="1" t="n">
+        <v>57.034</v>
+      </c>
+      <c r="J66" s="2" t="n">
+        <f aca="false">F66/I66</f>
+        <v>3.77178525090297</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F67" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I67" s="1" t="n">
+        <v>54.0377</v>
+      </c>
+      <c r="J67" s="2" t="n">
+        <f aca="false">F67/I67</f>
+        <v>3.9809244286859</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F68" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I68" s="1" t="n">
+        <v>52.7309</v>
+      </c>
+      <c r="J68" s="2" t="n">
+        <f aca="false">F68/I68</f>
+        <v>4.07958142189874</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F69" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I69" s="1" t="n">
+        <v>52.0343</v>
+      </c>
+      <c r="J69" s="2" t="n">
+        <f aca="false">F69/I69</f>
+        <v>4.1341960975741</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F70" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I70" s="1" t="n">
+        <v>53.8669</v>
+      </c>
+      <c r="J70" s="2" t="n">
+        <f aca="false">F70/I70</f>
+        <v>3.99354705765507</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F71" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I71" s="1" t="n">
+        <v>55.0645</v>
+      </c>
+      <c r="J71" s="2" t="n">
+        <f aca="false">F71/I71</f>
+        <v>3.90669124390488</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F72" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I72" s="1" t="n">
+        <v>56.5129</v>
+      </c>
+      <c r="J72" s="2" t="n">
+        <f aca="false">F72/I72</f>
+        <v>3.80656451889746</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I73" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F74" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I74" s="1" t="n">
+        <v>205.818</v>
+      </c>
+      <c r="J74" s="2" t="n">
+        <f aca="false">F74/I74</f>
+        <v>1.04519526960713</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F75" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I75" s="1" t="n">
+        <v>121.417</v>
+      </c>
+      <c r="J75" s="2" t="n">
+        <f aca="false">F75/I75</f>
+        <v>1.77174530749401</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F76" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I76" s="1" t="n">
+        <v>70.7402</v>
+      </c>
+      <c r="J76" s="2" t="n">
+        <f aca="false">F76/I76</f>
+        <v>3.04098659602319</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F77" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I77" s="1" t="n">
+        <v>52.0762</v>
+      </c>
+      <c r="J77" s="2" t="n">
+        <f aca="false">F77/I77</f>
+        <v>4.13086976392287</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F78" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I78" s="1" t="n">
+        <v>44.2202</v>
+      </c>
+      <c r="J78" s="2" t="n">
+        <f aca="false">F78/I78</f>
+        <v>4.86474507125703</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F79" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I79" s="1" t="n">
+        <v>39.9327</v>
+      </c>
+      <c r="J79" s="2" t="n">
+        <f aca="false">F79/I79</f>
+        <v>5.38706373473369</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F80" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I80" s="1" t="n">
+        <v>37.4258</v>
+      </c>
+      <c r="J80" s="2" t="n">
+        <f aca="false">F80/I80</f>
+        <v>5.74790652437623</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F81" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I81" s="1" t="n">
+        <v>34.4642</v>
+      </c>
+      <c r="J81" s="2" t="n">
+        <f aca="false">F81/I81</f>
+        <v>6.24183935794245</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F82" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I82" s="1" t="n">
+        <v>32.3932</v>
+      </c>
+      <c r="J82" s="2" t="n">
+        <f aca="false">F82/I82</f>
+        <v>6.64089994196313</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F83" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I83" s="1" t="n">
+        <v>58.5664</v>
+      </c>
+      <c r="J83" s="2" t="n">
+        <f aca="false">F83/I83</f>
+        <v>3.6730958365206</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F84" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I84" s="1" t="n">
+        <v>56.4868</v>
+      </c>
+      <c r="J84" s="2" t="n">
+        <f aca="false">F84/I84</f>
+        <v>3.80832336050192</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F85" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I85" s="1" t="n">
+        <v>54.0965</v>
+      </c>
+      <c r="J85" s="2" t="n">
+        <f aca="false">F85/I85</f>
+        <v>3.97659737690978</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F86" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I86" s="1" t="n">
+        <v>52.7344</v>
+      </c>
+      <c r="J86" s="2" t="n">
+        <f aca="false">F86/I86</f>
+        <v>4.07931065869717</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F87" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I87" s="1" t="n">
+        <v>52.6036</v>
+      </c>
+      <c r="J87" s="2" t="n">
+        <f aca="false">F87/I87</f>
+        <v>4.0894539537218</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F88" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I88" s="1" t="n">
+        <v>53.768</v>
+      </c>
+      <c r="J88" s="2" t="n">
+        <f aca="false">F88/I88</f>
+        <v>4.00089272429698</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F89" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I89" s="1" t="n">
+        <v>56.83</v>
+      </c>
+      <c r="J89" s="2" t="n">
+        <f aca="false">F89/I89</f>
+        <v>3.78532465247229</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F90" s="1" t="n">
+        <v>215.12</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I90" s="1" t="n">
+        <v>56.6126</v>
+      </c>
+      <c r="J90" s="2" t="n">
+        <f aca="false">F90/I90</f>
+        <v>3.79986080837128</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4420,5 +6547,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>